<commit_message>
:white_check_mark: added ecp and bv tests for cnp validation
</commit_message>
<xml_diff>
--- a/Doc/Lab1/Lab01_ReviewReport.xlsx
+++ b/Doc/Lab1/Lab01_ReviewReport.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Bia\College\3rdYear\2ndSem\UVSS\UVSS_OB\Doc\Lab1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC96B8ED-5ED2-4714-A4CC-C97E60E0076F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD56ADB5-EA84-4136-ACEF-15F3205F74AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{E71D69E0-07DD-42D7-891A-8925EB0A6792}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="42">
   <si>
     <t>Crt. No.</t>
   </si>
@@ -144,6 +144,24 @@
   </si>
   <si>
     <t>Es fehlten Anforderungen</t>
+  </si>
+  <si>
+    <t>habe list out of range verbessert</t>
+  </si>
+  <si>
+    <t xml:space="preserve">es gibt einige Serivces, </t>
+  </si>
+  <si>
+    <t>Die Image orientirung funktioniert nicht in alle Falle (roteste cele care sunt deja drepte), neue Orientierung Funktion implementiert</t>
+  </si>
+  <si>
+    <t>Ca si parametrii se primeste direct poza, nu linkul pozei</t>
+  </si>
+  <si>
+    <t>Alle Bedurfnisse der Nutzer wurden in Acht genommen</t>
+  </si>
+  <si>
+    <t>Die Services sind in verschiedene files implementiert</t>
   </si>
 </sst>
 </file>
@@ -527,7 +545,7 @@
   <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="117" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -611,6 +629,9 @@
       <c r="C4" t="s">
         <v>15</v>
       </c>
+      <c r="D4" t="s">
+        <v>40</v>
+      </c>
       <c r="F4" s="1" t="s">
         <v>5</v>
       </c>
@@ -628,6 +649,9 @@
       <c r="C5" t="s">
         <v>17</v>
       </c>
+      <c r="D5" t="s">
+        <v>41</v>
+      </c>
       <c r="F5" s="1" t="s">
         <v>6</v>
       </c>
@@ -645,6 +669,9 @@
       <c r="C6" t="s">
         <v>20</v>
       </c>
+      <c r="D6" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7">
@@ -656,6 +683,9 @@
       <c r="C7" t="s">
         <v>21</v>
       </c>
+      <c r="D7" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8">
@@ -667,6 +697,9 @@
       <c r="C8" t="s">
         <v>23</v>
       </c>
+      <c r="D8" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9">
@@ -688,6 +721,9 @@
       </c>
       <c r="C10" t="s">
         <v>27</v>
+      </c>
+      <c r="D10" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
:bulb: added ecp and bva comments
</commit_message>
<xml_diff>
--- a/Doc/Lab1/Lab01_ReviewReport.xlsx
+++ b/Doc/Lab1/Lab01_ReviewReport.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Bia\College\3rdYear\2ndSem\UVSS\UVSS_OB\Doc\Lab1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD56ADB5-EA84-4136-ACEF-15F3205F74AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{907DF06E-5E50-48A1-A03F-8DD204B1B609}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{E71D69E0-07DD-42D7-891A-8925EB0A6792}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="43">
   <si>
     <t>Crt. No.</t>
   </si>
@@ -162,6 +162,9 @@
   </si>
   <si>
     <t>Die Services sind in verschiedene files implementiert</t>
+  </si>
+  <si>
+    <t>Mit der Image orientation verbesserung gibt es wenigere Fehler</t>
   </si>
 </sst>
 </file>
@@ -545,7 +548,7 @@
   <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="117" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -711,6 +714,9 @@
       <c r="C9" t="s">
         <v>25</v>
       </c>
+      <c r="D9" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10">

</xml_diff>